<commit_message>
add logs for results examples
</commit_message>
<xml_diff>
--- a/QRE/200KB request 100ms delay log/200KB 100ms delay graphs.xlsx
+++ b/QRE/200KB request 100ms delay log/200KB 100ms delay graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Technion\Semester7\CommunicationProject\LCCN-QUIC-Spin-Bit\QRE\200KB request 100ms delay log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F8FE19-E469-48CB-88F1-5B0AD77C49A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7208691-4FBC-44E7-8DB8-D1C9A94438C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB6AD377-0B89-4236-984F-99EE797705C6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Wireshark edges S2C</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Wireshark initial</t>
+  </si>
+  <si>
+    <t>Extend:</t>
   </si>
 </sst>
 </file>
@@ -158,14 +161,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$7</c:f>
+              <c:f>Sheet1!$G$4:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>351.93899999999871</c:v>
                 </c:pt>
@@ -177,16 +192,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>752.41900000000044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>818.59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$7</c:f>
+              <c:f>Sheet1!$E$4:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>202.20899999999986</c:v>
                 </c:pt>
@@ -198,6 +216,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>142.5370000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>142.53700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -225,7 +246,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -440,6 +473,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time since connection started (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -502,6 +590,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RTT (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -552,7 +695,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -770,6 +913,9 @@
                 <c:pt idx="2">
                   <c:v>357.91</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>764.37599999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -786,6 +932,9 @@
                   <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>125</c:v>
                 </c:pt>
               </c:numCache>
@@ -830,6 +979,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time since connection started (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -893,6 +1097,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RTT (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -943,7 +1202,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2505,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307E7D64-3B7B-46C2-BC7F-5684721812EC}">
   <dimension ref="A3:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2617,6 +2876,15 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>142.53700000000001</v>
+      </c>
+      <c r="G8">
+        <v>818.59</v>
+      </c>
       <c r="I8">
         <v>120.88200000000001</v>
       </c>
@@ -2913,6 +3181,15 @@
       <c r="G37">
         <f>(F37-D41)*1000+F41</f>
         <v>764.37599999999918</v>
+      </c>
+      <c r="I37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37">
+        <v>125</v>
+      </c>
+      <c r="K37">
+        <v>764.37599999999998</v>
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.3">

</xml_diff>